<commit_message>
complete Tinh Thanh Quan Huyen Phuong Xa
</commit_message>
<xml_diff>
--- a/data_excel/QuanHuyen.xlsx
+++ b/data_excel/QuanHuyen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LH COMPUTER\Desktop\agri-tour-be\data_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LH COMPUTER\Desktop\seek-an-origin\data_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F003FE8-7C51-4DC1-8574-CC7312E132E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978C0C6B-4306-4370-AD45-BDD7FE324805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5004" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -4451,10 +4451,10 @@
     <t>description</t>
   </si>
   <si>
-    <t>id_parent</t>
-  </si>
-  <si>
-    <t>key</t>
+    <t>provinceId</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -4802,7 +4802,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>